<commit_message>
add dungeon item heoyao
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonItem.xlsx
+++ b/ConfigData/Xlsx/DungeonItem.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE5437ED-9CDE-4897-A146-11256519DD44}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="副本道具" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -75,13 +76,21 @@
   </si>
   <si>
     <t>魂石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑曜石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>diheiyao</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -752,7 +761,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -787,6 +796,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -834,7 +846,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -983,16 +1002,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:D5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A3:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:D6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:D6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:C4">
     <sortCondition ref="A3:A4"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id" dataDxfId="2"/>
-    <tableColumn id="2" name="Name" dataDxfId="1"/>
-    <tableColumn id="10" name="Ename"/>
-    <tableColumn id="3" name="Url" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ename"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Url" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1318,14 +1337,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1406,10 +1425,24 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
+        <v>46000003</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:D5">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
+  <conditionalFormatting sqref="B4:D6">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
can gain black stone by fight quests
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonItem.xlsx
+++ b/ConfigData/Xlsx/DungeonItem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE5437ED-9CDE-4897-A146-11256519DD44}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{88725242-081F-4739-99AD-E7B75AA1F985}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -84,6 +84,26 @@
   </si>
   <si>
     <t>diheiyao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Des</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以兑换卡牌的神奇石头</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务用到的特殊道具</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -761,7 +781,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -799,6 +819,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -846,7 +869,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -981,13 +1004,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1002,14 +1018,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:D6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:D6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:C4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:E6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:E6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:D4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{FFC6B731-C513-4B1E-8ED4-29814F22DFDA}" name="Des"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ename"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Url" dataDxfId="1"/>
   </tableColumns>
@@ -1338,24 +1355,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9" style="4"/>
-    <col min="6" max="6" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="4"/>
+    <col min="2" max="2" width="9" style="4"/>
+    <col min="3" max="3" width="25.5" style="4" customWidth="1"/>
+    <col min="4" max="6" width="9" style="4"/>
+    <col min="7" max="7" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1363,13 +1382,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1377,13 +1399,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1391,13 +1416,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>46000001</v>
       </c>
@@ -1405,13 +1433,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>46000002</v>
       </c>
@@ -1419,30 +1450,36 @@
         <v>14</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="E5" s="10" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>46000003</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:D6">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
+  <conditionalFormatting sqref="B4:E6">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>